<commit_message>
Adjustment based on the article for DiB
</commit_message>
<xml_diff>
--- a/_analysis/US8K_AV_metrics_CNN_2D.xlsx
+++ b/_analysis/US8K_AV_metrics_CNN_2D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andre_Florentino\03_particular\04_mestrado-FEI\97_master\_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3CF0DE-0B48-40A2-8CCA-FF1442DAA42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48ECFC9-7E4A-486D-8AB0-0A9AAEAC848C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="3" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="27">
   <si>
     <t>index</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Su_windowed</t>
+  </si>
+  <si>
+    <t>Considered in the article for DiB</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,6 +492,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,7 +716,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -772,14 +781,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -7354,8 +7367,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="205759" y="11784618"/>
-              <a:ext cx="14121928" cy="4585278"/>
+              <a:off x="196234" y="12260868"/>
+              <a:ext cx="13765693" cy="4775778"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8466,7 +8479,7 @@
     </format>
   </formats>
   <conditionalFormats count="18">
-    <conditionalFormat priority="2">
+    <conditionalFormat priority="21">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -8474,7 +8487,353 @@
               <x v="0"/>
             </reference>
             <reference field="1" count="1">
-              <x v="11"/>
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="5" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="20">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="5" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="19">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="5" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="18">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="3"/>
+            </reference>
+            <reference field="2" count="5" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="17">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="4"/>
+            </reference>
+            <reference field="2" count="5" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="16">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="5"/>
+            </reference>
+            <reference field="2" count="5" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="14">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="10" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="13">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="1"/>
+            </reference>
+            <reference field="2" count="10" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="12">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="2"/>
+            </reference>
+            <reference field="2" count="10" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="11">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="3"/>
+            </reference>
+            <reference field="2" count="10" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="10">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="4"/>
+            </reference>
+            <reference field="2" count="10" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="9">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="5"/>
+            </reference>
+            <reference field="2" count="10" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="7">
+      <pivotAreas count="1">
+        <pivotArea fieldPosition="0">
+          <references count="2">
+            <reference field="1" count="1">
+              <x v="6"/>
+            </reference>
+            <reference field="2" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="6">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="7"/>
+            </reference>
+            <reference field="2" count="10" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="5">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="8"/>
+            </reference>
+            <reference field="2" count="10" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="4">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1">
+              <x v="9"/>
             </reference>
             <reference field="2" count="10" selected="0">
               <x v="0"/>
@@ -8518,7 +8877,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="4">
+    <conditionalFormat priority="2">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -8526,7 +8885,7 @@
               <x v="0"/>
             </reference>
             <reference field="1" count="1">
-              <x v="9"/>
+              <x v="11"/>
             </reference>
             <reference field="2" count="10" selected="0">
               <x v="0"/>
@@ -8539,352 +8898,6 @@
               <x v="7"/>
               <x v="8"/>
               <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="5">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="8"/>
-            </reference>
-            <reference field="2" count="10" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="6">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="7"/>
-            </reference>
-            <reference field="2" count="10" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="7">
-      <pivotAreas count="1">
-        <pivotArea fieldPosition="0">
-          <references count="2">
-            <reference field="1" count="1">
-              <x v="6"/>
-            </reference>
-            <reference field="2" count="0" selected="0"/>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="9">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="5"/>
-            </reference>
-            <reference field="2" count="10" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="10">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="4"/>
-            </reference>
-            <reference field="2" count="10" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="11">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="3"/>
-            </reference>
-            <reference field="2" count="10" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="12">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="2"/>
-            </reference>
-            <reference field="2" count="10" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="13">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="1"/>
-            </reference>
-            <reference field="2" count="10" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="14">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="10" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-              <x v="7"/>
-              <x v="8"/>
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="16">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="5"/>
-            </reference>
-            <reference field="2" count="5" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="17">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="4"/>
-            </reference>
-            <reference field="2" count="5" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="18">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="3"/>
-            </reference>
-            <reference field="2" count="5" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="19">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="2"/>
-            </reference>
-            <reference field="2" count="5" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="20">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="1"/>
-            </reference>
-            <reference field="2" count="5" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="21">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="5" selected="0">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
             </reference>
           </references>
         </pivotArea>
@@ -9033,6 +9046,25 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1">
         <x14:conditionalFormats count="2">
+          <x14:conditionalFormat priority="8" id="{4275FAED-FBAC-4D01-8DE9-0D7255CD9300}">
+            <x14:pivotAreas count="1">
+              <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+                <references count="2">
+                  <reference field="4294967294" count="1" selected="0">
+                    <x v="0"/>
+                  </reference>
+                  <reference field="1" count="6">
+                    <x v="0"/>
+                    <x v="1"/>
+                    <x v="2"/>
+                    <x v="3"/>
+                    <x v="4"/>
+                    <x v="5"/>
+                  </reference>
+                </references>
+              </pivotArea>
+            </x14:pivotAreas>
+          </x14:conditionalFormat>
           <x14:conditionalFormat priority="1" id="{3A9D3AF8-726A-4989-81CB-D4128E8FAE4A}">
             <x14:pivotAreas count="1">
               <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -9047,25 +9079,6 @@
                     <x v="9"/>
                     <x v="10"/>
                     <x v="11"/>
-                  </reference>
-                </references>
-              </pivotArea>
-            </x14:pivotAreas>
-          </x14:conditionalFormat>
-          <x14:conditionalFormat priority="8" id="{4275FAED-FBAC-4D01-8DE9-0D7255CD9300}">
-            <x14:pivotAreas count="1">
-              <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-                <references count="2">
-                  <reference field="4294967294" count="1" selected="0">
-                    <x v="0"/>
-                  </reference>
-                  <reference field="1" count="6">
-                    <x v="0"/>
-                    <x v="1"/>
-                    <x v="2"/>
-                    <x v="3"/>
-                    <x v="4"/>
-                    <x v="5"/>
                   </reference>
                 </references>
               </pivotArea>
@@ -9382,34 +9395,34 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="21.44140625" customWidth="1"/>
-    <col min="13" max="13" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="21.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2"/>
     </row>
-    <row r="3" spans="2:18" s="7" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" s="7" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="C3" s="15" t="s">
         <v>19</v>
@@ -9432,13 +9445,13 @@
       <c r="Q3"/>
       <c r="R3"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="18"/>
       <c r="C5" s="19" t="s">
         <v>11</v>
@@ -9448,7 +9461,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>20</v>
       </c>
@@ -9462,21 +9475,25 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="26">
         <f>AVERAGEIF(raw_data!$C$2:$C$61,Comparison!B7,raw_data!$F$2:$F$61)</f>
         <v>0.82784970344753239</v>
       </c>
-      <c r="D7" s="17" cm="1">
+      <c r="D7" s="26" cm="1">
         <f t="array" ref="D7">_xlfn.STDEV.S(IF(raw_data!$C$2:$C$61=B7, raw_data!$F$2:$F$61))</f>
         <v>3.601469079383416E-2</v>
       </c>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>22</v>
       </c>
@@ -9490,7 +9507,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>23</v>
       </c>
@@ -9504,7 +9521,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
         <v>24</v>
       </c>
@@ -9518,96 +9535,100 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="28">
         <f>AVERAGEIF(raw_data!$C$2:$C$61,Comparison!B11,raw_data!$F$2:$F$61)</f>
         <v>0.80028823293293061</v>
       </c>
-      <c r="D11" s="24" cm="1">
+      <c r="D11" s="28" cm="1">
         <f t="array" ref="D11">_xlfn.STDEV.S(IF(raw_data!$C$2:$C$61=B11, raw_data!$F$2:$F$61))</f>
         <v>2.7126764295843944E-2</v>
       </c>
-      <c r="E11"/>
-    </row>
-    <row r="42" spans="2:12" s="20" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-    </row>
-    <row r="43" spans="2:12" s="20" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-    </row>
-    <row r="44" spans="2:12" s="20" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
-    </row>
-    <row r="45" spans="2:12" s="20" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
-      <c r="L45" s="25"/>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="27"/>
+    </row>
+    <row r="42" spans="2:12" s="20" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+    </row>
+    <row r="43" spans="2:12" s="20" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="24"/>
+    </row>
+    <row r="44" spans="2:12" s="20" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="24"/>
+    </row>
+    <row r="45" spans="2:12" s="20" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D48" s="21"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="21"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="21"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="21"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="21"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="21"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="21"/>
     </row>
   </sheetData>
@@ -9629,20 +9650,20 @@
   <dimension ref="B2:M199"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="11.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="5" customWidth="1"/>
-    <col min="10" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="11.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="5" customWidth="1"/>
+    <col min="10" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
@@ -9655,7 +9676,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
@@ -9693,7 +9714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
@@ -9731,7 +9752,7 @@
         <v>0.84137538663366329</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
@@ -9769,7 +9790,7 @@
         <v>0.82784970344753217</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
@@ -9807,7 +9828,7 @@
         <v>0.86286536315074325</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
@@ -9845,7 +9866,7 @@
         <v>0.85265372074970824</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
@@ -9883,7 +9904,7 @@
         <v>0.76980221302624985</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
@@ -9921,7 +9942,7 @@
         <v>0.80028823293293061</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
@@ -9959,13 +9980,13 @@
         <v>0.82580576999013811</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I11"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I12"/>
     </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -9975,7 +9996,7 @@
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
     </row>
-    <row r="51" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -9985,7 +10006,7 @@
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
     </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -9995,7 +10016,7 @@
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
     </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -10005,7 +10026,7 @@
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
     </row>
-    <row r="54" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -10015,7 +10036,7 @@
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
     </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -10025,7 +10046,7 @@
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
     </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -10035,7 +10056,7 @@
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
     </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -10045,7 +10066,7 @@
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
     </row>
-    <row r="58" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -10055,7 +10076,7 @@
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
     </row>
-    <row r="59" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -10065,7 +10086,7 @@
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
     </row>
-    <row r="60" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -10075,7 +10096,7 @@
       <c r="K60" s="8"/>
       <c r="L60" s="8"/>
     </row>
-    <row r="61" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -10085,7 +10106,7 @@
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
     </row>
-    <row r="62" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -10095,7 +10116,7 @@
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
     </row>
-    <row r="63" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -10105,7 +10126,7 @@
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
     </row>
-    <row r="64" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -10115,7 +10136,7 @@
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
     </row>
-    <row r="65" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -10125,7 +10146,7 @@
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
     </row>
-    <row r="66" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -10135,7 +10156,7 @@
       <c r="K66" s="8"/>
       <c r="L66" s="8"/>
     </row>
-    <row r="67" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -10145,7 +10166,7 @@
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
     </row>
-    <row r="68" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -10155,7 +10176,7 @@
       <c r="K68" s="8"/>
       <c r="L68" s="8"/>
     </row>
-    <row r="69" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -10165,7 +10186,7 @@
       <c r="K69" s="8"/>
       <c r="L69" s="8"/>
     </row>
-    <row r="70" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -10175,7 +10196,7 @@
       <c r="K70" s="8"/>
       <c r="L70" s="8"/>
     </row>
-    <row r="71" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -10185,7 +10206,7 @@
       <c r="K71" s="8"/>
       <c r="L71" s="8"/>
     </row>
-    <row r="72" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -10195,7 +10216,7 @@
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
     </row>
-    <row r="73" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -10205,7 +10226,7 @@
       <c r="K73" s="8"/>
       <c r="L73" s="8"/>
     </row>
-    <row r="74" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -10215,7 +10236,7 @@
       <c r="K74" s="8"/>
       <c r="L74" s="8"/>
     </row>
-    <row r="75" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -10225,7 +10246,7 @@
       <c r="K75" s="8"/>
       <c r="L75" s="8"/>
     </row>
-    <row r="76" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -10235,7 +10256,7 @@
       <c r="K76" s="8"/>
       <c r="L76" s="8"/>
     </row>
-    <row r="77" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -10245,7 +10266,7 @@
       <c r="K77" s="8"/>
       <c r="L77" s="8"/>
     </row>
-    <row r="78" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -10255,7 +10276,7 @@
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
     </row>
-    <row r="79" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -10265,7 +10286,7 @@
       <c r="K79" s="8"/>
       <c r="L79" s="8"/>
     </row>
-    <row r="80" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -10275,7 +10296,7 @@
       <c r="K80" s="8"/>
       <c r="L80" s="8"/>
     </row>
-    <row r="81" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -10285,7 +10306,7 @@
       <c r="K81" s="8"/>
       <c r="L81" s="8"/>
     </row>
-    <row r="82" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -10295,7 +10316,7 @@
       <c r="K82" s="8"/>
       <c r="L82" s="8"/>
     </row>
-    <row r="83" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -10305,7 +10326,7 @@
       <c r="K83" s="8"/>
       <c r="L83" s="8"/>
     </row>
-    <row r="84" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -10315,7 +10336,7 @@
       <c r="K84" s="8"/>
       <c r="L84" s="8"/>
     </row>
-    <row r="85" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -10325,7 +10346,7 @@
       <c r="K85" s="8"/>
       <c r="L85" s="8"/>
     </row>
-    <row r="86" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -10335,7 +10356,7 @@
       <c r="K86" s="8"/>
       <c r="L86" s="8"/>
     </row>
-    <row r="87" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -10345,7 +10366,7 @@
       <c r="K87" s="8"/>
       <c r="L87" s="8"/>
     </row>
-    <row r="88" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -10355,7 +10376,7 @@
       <c r="K88" s="8"/>
       <c r="L88" s="8"/>
     </row>
-    <row r="89" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -10365,7 +10386,7 @@
       <c r="K89" s="8"/>
       <c r="L89" s="8"/>
     </row>
-    <row r="90" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -10375,7 +10396,7 @@
       <c r="K90" s="8"/>
       <c r="L90" s="8"/>
     </row>
-    <row r="91" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -10385,148 +10406,148 @@
       <c r="K91" s="8"/>
       <c r="L91" s="8"/>
     </row>
-    <row r="93" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I93"/>
     </row>
-    <row r="94" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I94"/>
     </row>
-    <row r="95" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I95"/>
     </row>
-    <row r="96" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:12" x14ac:dyDescent="0.25">
       <c r="I96"/>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I97"/>
     </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I98"/>
     </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I99"/>
     </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I100"/>
     </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I101"/>
     </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I102"/>
     </row>
-    <row r="116" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K116" s="2"/>
     </row>
-    <row r="117" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K117" s="2"/>
     </row>
-    <row r="118" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K118" s="2"/>
     </row>
-    <row r="119" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K119" s="2"/>
     </row>
-    <row r="120" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K120" s="2"/>
     </row>
-    <row r="121" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K122" s="2"/>
     </row>
-    <row r="123" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K123" s="2"/>
     </row>
-    <row r="170" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I170"/>
     </row>
-    <row r="171" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I171"/>
     </row>
-    <row r="172" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I172"/>
     </row>
-    <row r="173" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I173"/>
     </row>
-    <row r="174" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I174"/>
     </row>
-    <row r="175" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I175"/>
     </row>
-    <row r="176" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I176"/>
     </row>
-    <row r="177" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I177"/>
     </row>
-    <row r="178" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I178"/>
     </row>
-    <row r="179" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I179"/>
     </row>
-    <row r="180" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I180"/>
     </row>
-    <row r="181" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I181"/>
     </row>
-    <row r="182" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I182"/>
     </row>
-    <row r="183" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I183"/>
     </row>
-    <row r="184" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I184"/>
     </row>
-    <row r="185" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I185"/>
     </row>
-    <row r="186" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I186"/>
     </row>
-    <row r="187" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I187"/>
     </row>
-    <row r="188" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I188"/>
     </row>
-    <row r="189" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I189"/>
     </row>
-    <row r="190" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I190"/>
     </row>
-    <row r="191" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I191"/>
     </row>
-    <row r="192" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I192"/>
     </row>
-    <row r="193" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I193"/>
     </row>
-    <row r="194" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I194"/>
     </row>
-    <row r="195" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I195"/>
     </row>
-    <row r="196" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I196"/>
     </row>
-    <row r="197" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I197"/>
     </row>
-    <row r="198" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I198"/>
     </row>
-    <row r="199" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I199"/>
     </row>
   </sheetData>
@@ -10809,25 +10830,25 @@
       <selection activeCell="P68" sqref="P68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10865,7 +10886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -10906,7 +10927,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -10947,7 +10968,7 @@
         <v>578125</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -10988,7 +11009,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -11029,7 +11050,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -11070,7 +11091,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -11111,7 +11132,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -11152,7 +11173,7 @@
         <v>359375</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -11193,7 +11214,7 @@
         <v>390625</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -11234,7 +11255,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -11275,7 +11296,7 @@
         <v>343.75</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -11316,7 +11337,7 @@
         <v>296875</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -11357,7 +11378,7 @@
         <v>234375</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -11398,7 +11419,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -11439,7 +11460,7 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -11480,7 +11501,7 @@
         <v>93.75</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -11521,7 +11542,7 @@
         <v>93.75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -11562,7 +11583,7 @@
         <v>234375</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -11603,7 +11624,7 @@
         <v>93.75</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -11644,7 +11665,7 @@
         <v>343.75</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -11685,7 +11706,7 @@
         <v>203125</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -11726,7 +11747,7 @@
         <v>2390625</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -11767,7 +11788,7 @@
         <v>1859375</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -11808,7 +11829,7 @@
         <v>2140625</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -11849,7 +11870,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -11890,7 +11911,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
@@ -11931,7 +11952,7 @@
         <v>2062.5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -11972,7 +11993,7 @@
         <v>1703125</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -12013,7 +12034,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>8</v>
       </c>
@@ -12054,7 +12075,7 @@
         <v>2203125</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9</v>
       </c>
@@ -12095,7 +12116,7 @@
         <v>1515625</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10</v>
       </c>
@@ -12136,7 +12157,7 @@
         <v>1562.5</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>11</v>
       </c>
@@ -12177,7 +12198,7 @@
         <v>1140625</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>12</v>
       </c>
@@ -12218,7 +12239,7 @@
         <v>1171875</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>13</v>
       </c>
@@ -12259,7 +12280,7 @@
         <v>703125</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>14</v>
       </c>
@@ -12300,7 +12321,7 @@
         <v>1109375</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>15</v>
       </c>
@@ -12341,7 +12362,7 @@
         <v>765625</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>16</v>
       </c>
@@ -12382,7 +12403,7 @@
         <v>781.25</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>17</v>
       </c>
@@ -12423,7 +12444,7 @@
         <v>718.75</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>18</v>
       </c>
@@ -12464,7 +12485,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>19</v>
       </c>
@@ -12505,7 +12526,7 @@
         <v>765625</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -12546,7 +12567,7 @@
         <v>1062.5</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -12587,7 +12608,7 @@
         <v>531.25</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -12628,7 +12649,7 @@
         <v>531.25</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -12669,7 +12690,7 @@
         <v>703125</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -12710,7 +12731,7 @@
         <v>421875</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5</v>
       </c>
@@ -12751,7 +12772,7 @@
         <v>703125</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>6</v>
       </c>
@@ -12792,7 +12813,7 @@
         <v>781.25</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -12833,7 +12854,7 @@
         <v>609375</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>8</v>
       </c>
@@ -12874,7 +12895,7 @@
         <v>578125</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>9</v>
       </c>
@@ -12915,7 +12936,7 @@
         <v>390625</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>10</v>
       </c>
@@ -12956,7 +12977,7 @@
         <v>390625</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>11</v>
       </c>
@@ -12997,7 +13018,7 @@
         <v>562.5</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>12</v>
       </c>
@@ -13038,7 +13059,7 @@
         <v>265625</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>13</v>
       </c>
@@ -13079,7 +13100,7 @@
         <v>296875</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>14</v>
       </c>
@@ -13120,7 +13141,7 @@
         <v>562.5</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>15</v>
       </c>
@@ -13161,7 +13182,7 @@
         <v>296875</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>16</v>
       </c>
@@ -13202,7 +13223,7 @@
         <v>578125</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>17</v>
       </c>
@@ -13243,7 +13264,7 @@
         <v>609375</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>18</v>
       </c>
@@ -13284,7 +13305,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>19</v>
       </c>

</xml_diff>